<commit_message>
full set of data
</commit_message>
<xml_diff>
--- a/myData/JHL beta gal data 2.5.2.xlsx
+++ b/myData/JHL beta gal data 2.5.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennylee/Desktop/research/Jenny_MutantSensitivity/betaGal-analysis/myData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9561C9C8-86CB-7942-8E57-5787D9FDE4CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F214356-9232-A844-8C2C-EEC7CC4D21D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="500" windowWidth="24920" windowHeight="14380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="500" windowWidth="24920" windowHeight="14380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -859,8 +859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N135"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79:I135"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3608,7 +3608,7 @@
   <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+      <selection activeCell="J1" sqref="J1:P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4806,7 +4806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>

</xml_diff>